<commit_message>
connected to DB,pictures saved in current directory...Everything is working
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -127,13 +127,13 @@
     <t>https://akam.cdn.jdmagicbox.com/intimages/us/jd_rwd/dtl_pg_img/gradient-result2.jpg</t>
   </si>
   <si>
-    <t>https://images2.jdmagicbox.com/uae/jdcatalogue/dubai/77/2013061677/catalogue/a8b1f7ed9ca7c791883ada40a6b0fef9.jpg?output-quality=100</t>
-  </si>
-  <si>
-    <t>https://images2.jdmagicbox.com/uae/jdcatalogue/abu_dhabi/88/2013123988/catalogue/e18ffdfba70cc9aceff9a07911af28d5.jpg?output-quality=100</t>
-  </si>
-  <si>
-    <t>https://images1.jdmagicbox.com/uae/jdcatalogue/abu_dhabi/77/nde0244705677/catalogue/3969920607d9a5e15a142f8f74c998a7.jpg?output-quality=100</t>
+    <t>https://images4.jdmagicbox.com/uae/jdcatalogue/dubai/77/2013061677/catalogue/a8b1f7ed9ca7c791883ada40a6b0fef9.jpg?output-quality=100</t>
+  </si>
+  <si>
+    <t>https://images3.jdmagicbox.com/uae/jdcatalogue/abu_dhabi/88/2013123988/catalogue/e18ffdfba70cc9aceff9a07911af28d5.jpg?output-quality=100</t>
+  </si>
+  <si>
+    <t>https://images3.jdmagicbox.com/uae/jdcatalogue/abu_dhabi/77/nde0244705677/catalogue/3969920607d9a5e15a142f8f74c998a7.jpg?output-quality=100</t>
   </si>
   <si>
     <t>near Bu Kadra</t>

</xml_diff>